<commit_message>
Board V1 - MK1 MCC update 2
</commit_message>
<xml_diff>
--- a/Boards/MK1/docs/PinOut.xlsx
+++ b/Boards/MK1/docs/PinOut.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\ACIM\FWLIB\main\Boards\MK1\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECDE357-3531-4705-84E4-DA81F09F85FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F283585-E0D9-444C-84DF-444754B94FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{743FF5B2-4EDE-46D0-BACB-F1D2176B51F7}"/>
+    <workbookView xWindow="-20610" yWindow="15" windowWidth="20730" windowHeight="11310" xr2:uid="{743FF5B2-4EDE-46D0-BACB-F1D2176B51F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="94">
   <si>
     <t>Ports</t>
   </si>
@@ -47,12 +50,6 @@
     <t>RA4</t>
   </si>
   <si>
-    <t>ADC</t>
-  </si>
-  <si>
-    <t>MC_IV_SEN</t>
-  </si>
-  <si>
     <t>RA8</t>
   </si>
   <si>
@@ -194,12 +191,6 @@
     <t>ENC_B</t>
   </si>
   <si>
-    <t>ENC_IDX</t>
-  </si>
-  <si>
-    <t>ENC_HOME</t>
-  </si>
-  <si>
     <t>RD5</t>
   </si>
   <si>
@@ -218,12 +209,6 @@
     <t>RG7</t>
   </si>
   <si>
-    <t>RG8</t>
-  </si>
-  <si>
-    <t>RG9</t>
-  </si>
-  <si>
     <t>FAULT</t>
   </si>
   <si>
@@ -233,12 +218,6 @@
     <t>QEIB</t>
   </si>
   <si>
-    <t>QEIIDX</t>
-  </si>
-  <si>
-    <t>QEIHOME</t>
-  </si>
-  <si>
     <t>PWM12</t>
   </si>
   <si>
@@ -266,9 +245,6 @@
     <t>Ngõ vào ADC đo dòng pha U</t>
   </si>
   <si>
-    <t>Ngõ vào ADC đo dòng pha V</t>
-  </si>
-  <si>
     <t>Ngõ vào ADC đo dòng tổng</t>
   </si>
   <si>
@@ -311,12 +287,6 @@
     <t>Ngõ ra cổng bất đồng bộ dùng hiển thị thông tin/ báo lỗi hệ thống lên máy tính. Tốc độ 115.200kbps</t>
   </si>
   <si>
-    <t>Encoder chân index (nếu có)</t>
-  </si>
-  <si>
-    <t>Encoder chân home (nếu có)</t>
-  </si>
-  <si>
     <t>Encoder chân B</t>
   </si>
   <si>
@@ -333,6 +303,24 @@
   </si>
   <si>
     <t>LED báo lỗi hệ thống</t>
+  </si>
+  <si>
+    <t>AN24</t>
+  </si>
+  <si>
+    <t>AN2</t>
+  </si>
+  <si>
+    <t>AN26</t>
+  </si>
+  <si>
+    <t>AN6</t>
+  </si>
+  <si>
+    <t>MC_IW_SEN</t>
+  </si>
+  <si>
+    <t>Ngõ vào ADC đo dòng pha W</t>
   </si>
 </sst>
 </file>
@@ -748,41 +736,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9723CA30-332C-4F7E-B81A-126FE63E3CC3}">
-  <dimension ref="A1:F25"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="89.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -796,18 +786,18 @@
         <v>2</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>3</v>
+        <v>88</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>4</v>
@@ -816,118 +806,118 @@
         <v>5</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>3</v>
+        <v>89</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>22</v>
@@ -936,190 +926,190 @@
         <v>23</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="E15" s="5" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
+        <v>50</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="C16" s="5" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
+        <v>4</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="D18" s="5" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>83</v>
@@ -1127,146 +1117,112 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>8</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
-        <v>47</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{9723CA30-332C-4F7E-B81A-126FE63E3CC3}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F23">
+      <sortCondition ref="E1"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="88" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>